<commit_message>
added aggregate row to mapping spreadsheet and pie chart age analysis
</commit_message>
<xml_diff>
--- a/Collections/AgeRangeMapping.xlsx
+++ b/Collections/AgeRangeMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swanson/Projects/Board_Game_Analysis/Collections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CA21BF-473D-E141-AD77-A9DFDD2F3C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558C3710-0918-BB4D-B087-1632E7DDCEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21180" yWindow="6400" windowWidth="27240" windowHeight="16440" xr2:uid="{8FA947F1-56D9-EB45-A11C-CF0F281CB0FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="56">
   <si>
     <t>bggrecagerange</t>
   </si>
@@ -189,13 +189,28 @@
   </si>
   <si>
     <t>25+</t>
+  </si>
+  <si>
+    <t>AggregateMapping</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>Preteens</t>
+  </si>
+  <si>
+    <t>Teens</t>
+  </si>
+  <si>
+    <t>Adults</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,6 +230,13 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -253,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -265,6 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,19 +622,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A205D8-79D1-FE45-8CE9-6B2FDA376D03}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,8 +646,11 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -634,8 +662,11 @@
         <f t="shared" ref="C2:C33" si="0">LEFT(B2, LEN(B2) - 1)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -646,8 +677,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -658,8 +692,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -670,8 +707,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -682,8 +722,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -695,8 +738,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -707,8 +753,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -719,8 +768,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -731,8 +783,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -743,8 +798,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -755,8 +813,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -768,8 +829,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -780,8 +844,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -792,8 +859,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -804,8 +874,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>4</v>
       </c>
@@ -816,8 +889,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -829,8 +905,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -841,8 +920,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -853,8 +935,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
@@ -865,8 +950,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -877,8 +965,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -889,8 +980,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -901,8 +995,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>5</v>
       </c>
@@ -913,8 +1010,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
@@ -926,8 +1026,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
@@ -938,8 +1041,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
@@ -950,8 +1056,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
@@ -962,8 +1071,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>25</v>
       </c>
@@ -974,8 +1086,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>6</v>
       </c>
@@ -986,8 +1101,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>7</v>
       </c>
@@ -998,8 +1116,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>27</v>
       </c>
@@ -1011,8 +1132,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>28</v>
       </c>
@@ -1020,11 +1144,14 @@
         <v>27</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" ref="C34:C65" si="1">LEFT(B34, LEN(B34) - 1)</f>
+        <f t="shared" ref="C34:C59" si="1">LEFT(B34, LEN(B34) - 1)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>29</v>
       </c>
@@ -1035,8 +1162,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>30</v>
       </c>
@@ -1047,8 +1177,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>8</v>
       </c>
@@ -1059,8 +1192,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>9</v>
       </c>
@@ -1071,8 +1207,11 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>32</v>
       </c>
@@ -1084,8 +1223,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>33</v>
       </c>
@@ -1096,8 +1238,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>34</v>
       </c>
@@ -1108,8 +1253,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>35</v>
       </c>
@@ -1120,8 +1268,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>10</v>
       </c>
@@ -1132,8 +1283,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>11</v>
       </c>
@@ -1144,8 +1298,11 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>37</v>
       </c>
@@ -1157,8 +1314,11 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>38</v>
       </c>
@@ -1169,8 +1329,11 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>39</v>
       </c>
@@ -1181,8 +1344,11 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>12</v>
       </c>
@@ -1193,8 +1359,11 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>13</v>
       </c>
@@ -1205,8 +1374,11 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
@@ -1218,8 +1390,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>42</v>
       </c>
@@ -1230,8 +1405,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>14</v>
       </c>
@@ -1242,8 +1420,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>15</v>
       </c>
@@ -1254,8 +1435,11 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>44</v>
       </c>
@@ -1267,8 +1451,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>16</v>
       </c>
@@ -1279,8 +1466,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>17</v>
       </c>
@@ -1291,8 +1481,11 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>46</v>
       </c>
@@ -1304,8 +1497,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>47</v>
       </c>
@@ -1316,8 +1512,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>18</v>
       </c>
@@ -1328,8 +1527,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>48</v>
       </c>
@@ -1339,8 +1541,11 @@
       <c r="C60" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>21</v>
       </c>
@@ -1350,8 +1555,11 @@
       <c r="C61" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>25</v>
       </c>
@@ -1360,6 +1568,9 @@
       </c>
       <c r="C62" s="4">
         <v>18</v>
+      </c>
+      <c r="D62" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrections to bar graph, leading/trailing spaces was causing the trouble
</commit_message>
<xml_diff>
--- a/Collections/AgeRangeMapping.xlsx
+++ b/Collections/AgeRangeMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swanson/Projects/Board_Game_Analysis/Collections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558C3710-0918-BB4D-B087-1632E7DDCEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9949B92-2E4C-5140-8D3D-56D15D635793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="6400" windowWidth="27240" windowHeight="16440" xr2:uid="{8FA947F1-56D9-EB45-A11C-CF0F281CB0FB}"/>
+    <workbookView xWindow="21180" yWindow="6400" windowWidth="34120" windowHeight="19880" xr2:uid="{8FA947F1-56D9-EB45-A11C-CF0F281CB0FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,16 +194,16 @@
     <t>AggregateMapping</t>
   </si>
   <si>
-    <t>Kids</t>
-  </si>
-  <si>
-    <t>Preteens</t>
-  </si>
-  <si>
-    <t>Teens</t>
-  </si>
-  <si>
-    <t>Adults</t>
+    <t>Kids (2-7)</t>
+  </si>
+  <si>
+    <t>Preteens (8-12)</t>
+  </si>
+  <si>
+    <t>Teens (13-17)</t>
+  </si>
+  <si>
+    <t>Adults (18+)</t>
   </si>
 </sst>
 </file>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A205D8-79D1-FE45-8CE9-6B2FDA376D03}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57:D62"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>